<commit_message>
few changes made sofar
</commit_message>
<xml_diff>
--- a/uploads/class_type.xlsx
+++ b/uploads/class_type.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29530"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\float_working2\data\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A73F84D-A78F-4B51-8E89-EECC3105A589}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{482E63BB-337B-47C4-B1DE-E088B1AA6D3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="136">
   <si>
     <t>subject</t>
   </si>
@@ -349,9 +349,6 @@
     <t>BEE</t>
   </si>
   <si>
-    <t>PROJ[TELAB/GTLAB]</t>
-  </si>
-  <si>
     <t>CADA LAB/TE-II LAB</t>
   </si>
   <si>
@@ -422,13 +419,22 @@
   </si>
   <si>
     <t xml:space="preserve">PS Lab/PE Lab          </t>
+  </si>
+  <si>
+    <t>Activity Hour</t>
+  </si>
+  <si>
+    <t>PROJ[TE LAB/GT LAB]</t>
+  </si>
+  <si>
+    <t>Project</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -440,6 +446,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -480,7 +493,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -488,6 +501,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -792,10 +806,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B135"/>
+  <dimension ref="A1:B137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" zoomScale="85" workbookViewId="0">
-      <selection activeCell="C122" sqref="C122"/>
+    <sheetView tabSelected="1" topLeftCell="A111" zoomScale="85" workbookViewId="0">
+      <selection activeCell="B138" sqref="B138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1614,7 +1628,7 @@
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B102" t="s">
         <v>12</v>
@@ -1622,7 +1636,7 @@
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B103" t="s">
         <v>12</v>
@@ -1630,7 +1644,7 @@
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B104" t="s">
         <v>12</v>
@@ -1646,7 +1660,7 @@
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B106" t="s">
         <v>12</v>
@@ -1654,7 +1668,7 @@
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B107" t="s">
         <v>12</v>
@@ -1662,7 +1676,7 @@
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B108" t="s">
         <v>12</v>
@@ -1670,7 +1684,7 @@
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B109" t="s">
         <v>12</v>
@@ -1678,7 +1692,7 @@
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B110" t="s">
         <v>12</v>
@@ -1694,7 +1708,7 @@
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B112" t="s">
         <v>12</v>
@@ -1710,7 +1724,7 @@
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B114" t="s">
         <v>12</v>
@@ -1718,7 +1732,7 @@
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B115" t="s">
         <v>12</v>
@@ -1726,7 +1740,7 @@
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B116" t="s">
         <v>12</v>
@@ -1734,7 +1748,7 @@
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B117" t="s">
         <v>12</v>
@@ -1742,7 +1756,7 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B118" t="s">
         <v>12</v>
@@ -1750,7 +1764,7 @@
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B119" t="s">
         <v>12</v>
@@ -1758,7 +1772,7 @@
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B120" t="s">
         <v>12</v>
@@ -1766,7 +1780,7 @@
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B121" t="s">
         <v>12</v>
@@ -1774,7 +1788,7 @@
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B122" t="s">
         <v>12</v>
@@ -1782,7 +1796,7 @@
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A123" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B123" t="s">
         <v>12</v>
@@ -1806,7 +1820,7 @@
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B126" t="s">
         <v>12</v>
@@ -1830,7 +1844,7 @@
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>109</v>
+        <v>134</v>
       </c>
       <c r="B129" t="s">
         <v>12</v>
@@ -1838,7 +1852,7 @@
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B130" t="s">
         <v>12</v>
@@ -1846,7 +1860,7 @@
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B131" t="s">
         <v>12</v>
@@ -1854,7 +1868,7 @@
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B132" t="s">
         <v>12</v>
@@ -1862,7 +1876,7 @@
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B133" t="s">
         <v>12</v>
@@ -1878,9 +1892,25 @@
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B135" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A136" t="s">
+        <v>133</v>
+      </c>
+      <c r="B136" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A137" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B137" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>